<commit_message>
[dev_company]  full dev_company with tests
</commit_message>
<xml_diff>
--- a/menu.xlsx
+++ b/menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silence\PycharmProjects\Web_Menu_DA\Web_Menu_DA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D862677-7A06-44B4-8A31-EEB0735A4DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B52274C-F545-44F5-8535-6963A0D3C52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3AFCCFBC-1BFD-42C5-8BE3-C448F22DF91F}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Аркуш2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="84">
   <si>
     <t>Технічне завдання “Online menu”</t>
   </si>
@@ -287,15 +288,6 @@
   </si>
   <si>
     <t>owner_expireed time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python manage.py makemigrations </t>
-  </si>
-  <si>
-    <t xml:space="preserve">python .\manage.py makemigrations </t>
-  </si>
-  <si>
-    <t>python .\manage.py migrate</t>
   </si>
 </sst>
 </file>
@@ -965,10 +957,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5FA9B6-43F9-4054-8D88-CDBA25EF1BA5}">
-  <dimension ref="B1:Q53"/>
+  <dimension ref="B1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -985,17 +977,17 @@
       <c r="K1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="7" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="L2" t="s">
+      <c r="L2" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L3" t="s">
+      <c r="L3" s="7" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1003,7 +995,7 @@
       <c r="G4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="7" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1021,7 +1013,7 @@
         <v>81</v>
       </c>
       <c r="H5" s="10"/>
-      <c r="L5" t="s">
+      <c r="L5" s="7" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1042,7 +1034,7 @@
         <v>81</v>
       </c>
       <c r="H6" s="10"/>
-      <c r="L6" t="s">
+      <c r="L6" s="7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1053,19 +1045,19 @@
       <c r="L7" t="s">
         <v>56</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" s="7" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1089,11 +1081,14 @@
       <c r="L8" t="s">
         <v>62</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="7" t="s">
         <v>64</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1110,16 +1105,13 @@
         <v>81</v>
       </c>
       <c r="H9" s="10"/>
-      <c r="L9" t="s">
-        <v>65</v>
+      <c r="L9" s="7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G10" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="L10" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="11" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1470,21 +1462,6 @@
     <row r="46" spans="3:14" x14ac:dyDescent="0.3">
       <c r="L46" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I51" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I52" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I53" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[dev_location] final location + tests
</commit_message>
<xml_diff>
--- a/menu.xlsx
+++ b/menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silence\PycharmProjects\Web_Menu_DA\Web_Menu_DA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B52274C-F545-44F5-8535-6963A0D3C52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4007A9-EFBE-44C4-B347-9A6A09589D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3AFCCFBC-1BFD-42C5-8BE3-C448F22DF91F}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Аркуш2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -959,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5FA9B6-43F9-4054-8D88-CDBA25EF1BA5}">
   <dimension ref="B1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1181,24 +1180,24 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I19" t="s">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="L18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I20" t="s">
         <v>72</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J20" t="s">
         <v>73</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K20" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L20" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="L20" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="21" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1229,7 +1228,7 @@
         <v>48</v>
       </c>
       <c r="L22" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1243,7 +1242,7 @@
         <v>48</v>
       </c>
       <c r="L23" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1260,7 +1259,7 @@
         <v>48</v>
       </c>
       <c r="L24" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
[product] product + tests
</commit_message>
<xml_diff>
--- a/menu.xlsx
+++ b/menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silence\PycharmProjects\Web_Menu_DA\Web_Menu_DA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4007A9-EFBE-44C4-B347-9A6A09589D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5768873-8188-4C6E-BBD4-0C616EA2124C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3AFCCFBC-1BFD-42C5-8BE3-C448F22DF91F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="95">
   <si>
     <t>Технічне завдання “Online menu”</t>
   </si>
@@ -287,13 +287,46 @@
   </si>
   <si>
     <t>owner_expireed time</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>product_id</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>buhlo</t>
+  </si>
+  <si>
+    <t>vodka</t>
+  </si>
+  <si>
+    <t>beer</t>
+  </si>
+  <si>
+    <t>meat</t>
+  </si>
+  <si>
+    <t>kovbasa</t>
+  </si>
+  <si>
+    <t>kotleta</t>
+  </si>
+  <si>
+    <t>breakfast</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,6 +354,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -336,7 +377,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -359,11 +400,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -387,6 +508,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
@@ -956,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5FA9B6-43F9-4054-8D88-CDBA25EF1BA5}">
-  <dimension ref="B1:Q46"/>
+  <dimension ref="B1:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="P58" sqref="P58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -968,6 +1101,7 @@
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
     <col min="15" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1463,6 +1597,160 @@
         <v>80</v>
       </c>
     </row>
+    <row r="50" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B51" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" s="13"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="13"/>
+      <c r="K51" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="L51" s="13"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B52" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="G52" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="K52" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="L52" s="16"/>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B53" s="14">
+        <v>1</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E53" s="14"/>
+      <c r="F53" s="15">
+        <v>1</v>
+      </c>
+      <c r="G53" s="16">
+        <v>1</v>
+      </c>
+      <c r="K53" s="14">
+        <v>1</v>
+      </c>
+      <c r="L53" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B54" s="14">
+        <v>2</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="E54" s="14"/>
+      <c r="F54" s="15">
+        <v>1</v>
+      </c>
+      <c r="G54" s="16">
+        <v>2</v>
+      </c>
+      <c r="K54" s="14">
+        <v>2</v>
+      </c>
+      <c r="L54" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B55" s="14">
+        <v>3</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E55" s="20"/>
+      <c r="F55" s="21">
+        <v>1</v>
+      </c>
+      <c r="G55" s="22">
+        <v>3</v>
+      </c>
+      <c r="K55" s="14"/>
+      <c r="L55" s="16"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B56" s="14"/>
+      <c r="C56" s="16"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="15">
+        <v>1</v>
+      </c>
+      <c r="G56" s="16">
+        <v>4</v>
+      </c>
+      <c r="K56" s="14"/>
+      <c r="L56" s="16"/>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B57" s="14"/>
+      <c r="C57" s="16"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="15">
+        <v>2</v>
+      </c>
+      <c r="G57" s="16">
+        <v>5</v>
+      </c>
+      <c r="K57" s="14">
+        <v>5</v>
+      </c>
+      <c r="L57" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B58" s="14"/>
+      <c r="C58" s="16"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="15">
+        <v>2</v>
+      </c>
+      <c r="G58" s="16">
+        <v>6</v>
+      </c>
+      <c r="K58" s="14">
+        <v>6</v>
+      </c>
+      <c r="L58" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="17"/>
+      <c r="C59" s="19"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="18">
+        <v>3</v>
+      </c>
+      <c r="G59" s="19">
+        <v>1</v>
+      </c>
+      <c r="K59" s="17"/>
+      <c r="L59" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>